<commit_message>
added slv4 in component in sub system
</commit_message>
<xml_diff>
--- a/my1stProject/apb_subsystem/apb_subsystem.xlsx
+++ b/my1stProject/apb_subsystem/apb_subsystem.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="19440" windowHeight="7635" tabRatio="820"/>
+    <workbookView xWindow="0" yWindow="120" windowWidth="19440" windowHeight="7635" tabRatio="820" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="9" r:id="rId1"/>
@@ -188,7 +188,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="511">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="515">
   <si>
     <t>Component Name</t>
   </si>
@@ -1831,6 +1831,18 @@
   </si>
   <si>
     <t>ex_ambaAHB_hprot[3:0]</t>
+  </si>
+  <si>
+    <t>i_apbbus_slv4</t>
+  </si>
+  <si>
+    <t>i_apbbus_slv4_paddr</t>
+  </si>
+  <si>
+    <t>i_apbbus_slv4_pwdata</t>
+  </si>
+  <si>
+    <t>i_apbbus_slv4_prdata</t>
   </si>
 </sst>
 </file>
@@ -2937,10 +2949,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3281,7 +3293,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3291,7 +3303,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
@@ -6000,9 +6012,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6667,7 +6679,7 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="15.75" thickBot="1">
-      <c r="B3" s="159"/>
+      <c r="B3" s="158"/>
       <c r="C3" s="112"/>
       <c r="D3" s="113"/>
       <c r="E3" s="114"/>
@@ -6681,8 +6693,8 @@
       <c r="M3" s="118"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" thickBot="1">
-      <c r="B4" s="159"/>
-      <c r="C4" s="159"/>
+      <c r="B4" s="158"/>
+      <c r="C4" s="158"/>
       <c r="D4" s="160"/>
       <c r="E4" s="161"/>
       <c r="F4" s="115"/>
@@ -6695,8 +6707,8 @@
       <c r="M4" s="118"/>
     </row>
     <row r="5" spans="1:13" ht="15.75" thickBot="1">
-      <c r="B5" s="159"/>
-      <c r="C5" s="159"/>
+      <c r="B5" s="158"/>
+      <c r="C5" s="158"/>
       <c r="D5" s="160"/>
       <c r="E5" s="161"/>
       <c r="F5" s="115"/>
@@ -6709,8 +6721,8 @@
       <c r="M5" s="118"/>
     </row>
     <row r="6" spans="1:13" ht="15.75" thickBot="1">
-      <c r="B6" s="159"/>
-      <c r="C6" s="159"/>
+      <c r="B6" s="158"/>
+      <c r="C6" s="158"/>
       <c r="D6" s="160"/>
       <c r="E6" s="161"/>
       <c r="F6" s="115"/>
@@ -6723,8 +6735,8 @@
       <c r="M6" s="118"/>
     </row>
     <row r="7" spans="1:13" ht="15.75" thickBot="1">
-      <c r="B7" s="159"/>
-      <c r="C7" s="159"/>
+      <c r="B7" s="158"/>
+      <c r="C7" s="158"/>
       <c r="D7" s="160"/>
       <c r="E7" s="161"/>
       <c r="F7" s="115"/>
@@ -6737,8 +6749,8 @@
       <c r="M7" s="118"/>
     </row>
     <row r="8" spans="1:13" ht="15.75" thickBot="1">
-      <c r="B8" s="159"/>
-      <c r="C8" s="159"/>
+      <c r="B8" s="158"/>
+      <c r="C8" s="158"/>
       <c r="D8" s="160"/>
       <c r="E8" s="161"/>
       <c r="F8" s="115"/>
@@ -6751,7 +6763,7 @@
       <c r="M8" s="124"/>
     </row>
     <row r="9" spans="1:13" ht="15.75" thickBot="1">
-      <c r="B9" s="159"/>
+      <c r="B9" s="158"/>
       <c r="C9" s="92"/>
       <c r="D9" s="113"/>
       <c r="E9" s="114"/>
@@ -6765,7 +6777,7 @@
       <c r="M9" s="124"/>
     </row>
     <row r="10" spans="1:13" ht="15.75" thickBot="1">
-      <c r="B10" s="159"/>
+      <c r="B10" s="158"/>
       <c r="C10" s="112"/>
       <c r="D10" s="113"/>
       <c r="E10" s="114"/>
@@ -6779,7 +6791,7 @@
       <c r="M10" s="113"/>
     </row>
     <row r="11" spans="1:13" ht="15.75" thickBot="1">
-      <c r="B11" s="159"/>
+      <c r="B11" s="158"/>
       <c r="C11" s="126"/>
       <c r="D11" s="118"/>
       <c r="E11" s="127"/>
@@ -6793,8 +6805,8 @@
       <c r="M11" s="118"/>
     </row>
     <row r="12" spans="1:13" ht="15.75" thickBot="1">
-      <c r="B12" s="158"/>
-      <c r="C12" s="159"/>
+      <c r="B12" s="159"/>
+      <c r="C12" s="158"/>
       <c r="D12" s="160"/>
       <c r="E12" s="114"/>
       <c r="F12" s="115"/>
@@ -6807,8 +6819,8 @@
       <c r="M12" s="124"/>
     </row>
     <row r="13" spans="1:13" ht="15.75" thickBot="1">
-      <c r="B13" s="158"/>
-      <c r="C13" s="159"/>
+      <c r="B13" s="159"/>
+      <c r="C13" s="158"/>
       <c r="D13" s="160"/>
       <c r="E13" s="114"/>
       <c r="F13" s="115"/>
@@ -6821,8 +6833,8 @@
       <c r="M13" s="124"/>
     </row>
     <row r="14" spans="1:13" ht="15.75" thickBot="1">
-      <c r="B14" s="158"/>
-      <c r="C14" s="159"/>
+      <c r="B14" s="159"/>
+      <c r="C14" s="158"/>
       <c r="D14" s="160"/>
       <c r="E14" s="114"/>
       <c r="F14" s="115"/>
@@ -6835,8 +6847,8 @@
       <c r="M14" s="124"/>
     </row>
     <row r="15" spans="1:13" ht="15.75" thickBot="1">
-      <c r="B15" s="158"/>
-      <c r="C15" s="159"/>
+      <c r="B15" s="159"/>
+      <c r="C15" s="158"/>
       <c r="D15" s="160"/>
       <c r="E15" s="114"/>
       <c r="F15" s="115"/>
@@ -6849,8 +6861,8 @@
       <c r="M15" s="124"/>
     </row>
     <row r="16" spans="1:13" ht="15.75" thickBot="1">
-      <c r="B16" s="158"/>
-      <c r="C16" s="159"/>
+      <c r="B16" s="159"/>
+      <c r="C16" s="158"/>
       <c r="D16" s="160"/>
       <c r="E16" s="114"/>
       <c r="F16" s="115"/>
@@ -6863,8 +6875,8 @@
       <c r="M16" s="124"/>
     </row>
     <row r="17" spans="2:13" ht="15.75" thickBot="1">
-      <c r="B17" s="158"/>
-      <c r="C17" s="159"/>
+      <c r="B17" s="159"/>
+      <c r="C17" s="158"/>
       <c r="D17" s="160"/>
       <c r="E17" s="114"/>
       <c r="F17" s="115"/>
@@ -6877,8 +6889,8 @@
       <c r="M17" s="124"/>
     </row>
     <row r="18" spans="2:13" ht="15.75" thickBot="1">
-      <c r="B18" s="158"/>
-      <c r="C18" s="159"/>
+      <c r="B18" s="159"/>
+      <c r="C18" s="158"/>
       <c r="D18" s="160"/>
       <c r="E18" s="114"/>
       <c r="F18" s="115"/>
@@ -6891,8 +6903,8 @@
       <c r="M18" s="124"/>
     </row>
     <row r="19" spans="2:13" ht="15.75" thickBot="1">
-      <c r="B19" s="158"/>
-      <c r="C19" s="159"/>
+      <c r="B19" s="159"/>
+      <c r="C19" s="158"/>
       <c r="D19" s="160"/>
       <c r="E19" s="114"/>
       <c r="F19" s="115"/>
@@ -6948,6 +6960,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="C16:C19"/>
+    <mergeCell ref="D16:D19"/>
+    <mergeCell ref="B3:B9"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="D4:D6"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="B12:B15"/>
@@ -6958,12 +6976,6 @@
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="E7:E8"/>
-    <mergeCell ref="B16:B19"/>
-    <mergeCell ref="C16:C19"/>
-    <mergeCell ref="D16:D19"/>
-    <mergeCell ref="B3:B9"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="D4:D6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7270,11 +7282,11 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H54"/>
+  <dimension ref="A1:H57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F40" sqref="F40"/>
+      <pane ySplit="2" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7584,7 +7596,7 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="17" t="s">
-        <v>455</v>
+        <v>511</v>
       </c>
       <c r="B22" s="14"/>
       <c r="C22" s="7"/>
@@ -7601,7 +7613,7 @@
         <v>456</v>
       </c>
       <c r="D23" s="87" t="s">
-        <v>457</v>
+        <v>512</v>
       </c>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
@@ -7615,7 +7627,7 @@
         <v>458</v>
       </c>
       <c r="D24" s="87" t="s">
-        <v>459</v>
+        <v>491</v>
       </c>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
@@ -7629,7 +7641,7 @@
         <v>460</v>
       </c>
       <c r="D25" s="87" t="s">
-        <v>461</v>
+        <v>492</v>
       </c>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
@@ -7643,7 +7655,7 @@
         <v>462</v>
       </c>
       <c r="D26" s="87" t="s">
-        <v>463</v>
+        <v>513</v>
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
@@ -7657,7 +7669,7 @@
         <v>464</v>
       </c>
       <c r="D27" s="87" t="s">
-        <v>465</v>
+        <v>490</v>
       </c>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
@@ -7671,7 +7683,7 @@
         <v>466</v>
       </c>
       <c r="D28" s="87" t="s">
-        <v>467</v>
+        <v>514</v>
       </c>
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
@@ -7708,7 +7720,7 @@
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="17" t="s">
-        <v>470</v>
+        <v>455</v>
       </c>
       <c r="B31" s="14"/>
       <c r="C31" s="87"/>
@@ -7725,7 +7737,7 @@
         <v>456</v>
       </c>
       <c r="D32" s="87" t="s">
-        <v>471</v>
+        <v>457</v>
       </c>
       <c r="E32" s="7"/>
       <c r="F32" s="7"/>
@@ -7739,7 +7751,7 @@
         <v>458</v>
       </c>
       <c r="D33" s="87" t="s">
-        <v>472</v>
+        <v>459</v>
       </c>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
@@ -7753,7 +7765,7 @@
         <v>460</v>
       </c>
       <c r="D34" s="87" t="s">
-        <v>473</v>
+        <v>461</v>
       </c>
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>
@@ -7767,7 +7779,7 @@
         <v>462</v>
       </c>
       <c r="D35" s="87" t="s">
-        <v>474</v>
+        <v>463</v>
       </c>
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
@@ -7781,7 +7793,7 @@
         <v>464</v>
       </c>
       <c r="D36" s="87" t="s">
-        <v>475</v>
+        <v>465</v>
       </c>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
@@ -7795,7 +7807,7 @@
         <v>466</v>
       </c>
       <c r="D37" s="87" t="s">
-        <v>476</v>
+        <v>467</v>
       </c>
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
@@ -7832,7 +7844,7 @@
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="17" t="s">
-        <v>477</v>
+        <v>470</v>
       </c>
       <c r="B40" s="14"/>
       <c r="C40" s="87"/>
@@ -7849,7 +7861,7 @@
         <v>456</v>
       </c>
       <c r="D41" s="87" t="s">
-        <v>478</v>
+        <v>471</v>
       </c>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
@@ -7863,7 +7875,7 @@
         <v>458</v>
       </c>
       <c r="D42" s="87" t="s">
-        <v>479</v>
+        <v>472</v>
       </c>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
@@ -7877,7 +7889,7 @@
         <v>460</v>
       </c>
       <c r="D43" s="87" t="s">
-        <v>480</v>
+        <v>473</v>
       </c>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
@@ -7891,7 +7903,7 @@
         <v>462</v>
       </c>
       <c r="D44" s="87" t="s">
-        <v>481</v>
+        <v>474</v>
       </c>
       <c r="E44" s="7"/>
       <c r="F44" s="7"/>
@@ -7905,7 +7917,7 @@
         <v>464</v>
       </c>
       <c r="D45" s="87" t="s">
-        <v>482</v>
+        <v>475</v>
       </c>
       <c r="E45" s="7"/>
       <c r="F45" s="7"/>
@@ -7919,7 +7931,7 @@
         <v>466</v>
       </c>
       <c r="D46" s="87" t="s">
-        <v>483</v>
+        <v>476</v>
       </c>
       <c r="E46" s="7"/>
       <c r="F46" s="7"/>
@@ -7955,7 +7967,9 @@
       <c r="H48" s="18"/>
     </row>
     <row r="49" spans="1:8">
-      <c r="A49" s="17"/>
+      <c r="A49" s="17" t="s">
+        <v>477</v>
+      </c>
       <c r="B49" s="14"/>
       <c r="C49" s="7"/>
       <c r="D49" s="7"/>
@@ -7967,8 +7981,12 @@
     <row r="50" spans="1:8">
       <c r="A50" s="17"/>
       <c r="B50" s="14"/>
-      <c r="C50" s="7"/>
-      <c r="D50" s="7"/>
+      <c r="C50" s="87" t="s">
+        <v>456</v>
+      </c>
+      <c r="D50" s="87" t="s">
+        <v>478</v>
+      </c>
       <c r="E50" s="7"/>
       <c r="F50" s="7"/>
       <c r="G50" s="7"/>
@@ -7977,8 +7995,12 @@
     <row r="51" spans="1:8">
       <c r="A51" s="17"/>
       <c r="B51" s="14"/>
-      <c r="C51" s="7"/>
-      <c r="D51" s="7"/>
+      <c r="C51" s="87" t="s">
+        <v>458</v>
+      </c>
+      <c r="D51" s="87" t="s">
+        <v>479</v>
+      </c>
       <c r="E51" s="7"/>
       <c r="F51" s="7"/>
       <c r="G51" s="7"/>
@@ -7987,8 +8009,12 @@
     <row r="52" spans="1:8">
       <c r="A52" s="17"/>
       <c r="B52" s="14"/>
-      <c r="C52" s="7"/>
-      <c r="D52" s="7"/>
+      <c r="C52" s="87" t="s">
+        <v>460</v>
+      </c>
+      <c r="D52" s="87" t="s">
+        <v>480</v>
+      </c>
       <c r="E52" s="7"/>
       <c r="F52" s="7"/>
       <c r="G52" s="7"/>
@@ -7997,8 +8023,12 @@
     <row r="53" spans="1:8">
       <c r="A53" s="17"/>
       <c r="B53" s="14"/>
-      <c r="C53" s="7"/>
-      <c r="D53" s="7"/>
+      <c r="C53" s="87" t="s">
+        <v>462</v>
+      </c>
+      <c r="D53" s="87" t="s">
+        <v>481</v>
+      </c>
       <c r="E53" s="7"/>
       <c r="F53" s="7"/>
       <c r="G53" s="7"/>
@@ -8007,12 +8037,58 @@
     <row r="54" spans="1:8">
       <c r="A54" s="17"/>
       <c r="B54" s="14"/>
-      <c r="C54" s="7"/>
-      <c r="D54" s="7"/>
+      <c r="C54" s="87" t="s">
+        <v>464</v>
+      </c>
+      <c r="D54" s="87" t="s">
+        <v>482</v>
+      </c>
       <c r="E54" s="7"/>
       <c r="F54" s="7"/>
       <c r="G54" s="7"/>
       <c r="H54" s="18"/>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55" s="17"/>
+      <c r="B55" s="14"/>
+      <c r="C55" s="87" t="s">
+        <v>466</v>
+      </c>
+      <c r="D55" s="87" t="s">
+        <v>483</v>
+      </c>
+      <c r="E55" s="7"/>
+      <c r="F55" s="7"/>
+      <c r="G55" s="7"/>
+      <c r="H55" s="18"/>
+    </row>
+    <row r="56" spans="1:8">
+      <c r="A56" s="17"/>
+      <c r="B56" s="14"/>
+      <c r="C56" s="87" t="s">
+        <v>468</v>
+      </c>
+      <c r="D56" s="87" t="s">
+        <v>452</v>
+      </c>
+      <c r="E56" s="7"/>
+      <c r="F56" s="7"/>
+      <c r="G56" s="7"/>
+      <c r="H56" s="18"/>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57" s="17"/>
+      <c r="B57" s="14"/>
+      <c r="C57" s="87" t="s">
+        <v>469</v>
+      </c>
+      <c r="D57" s="87" t="s">
+        <v>454</v>
+      </c>
+      <c r="E57" s="7"/>
+      <c r="F57" s="7"/>
+      <c r="G57" s="7"/>
+      <c r="H57" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>